<commit_message>
new transfer to uts
</commit_message>
<xml_diff>
--- a/ph_distr_direct_60deg.xlsx
+++ b/ph_distr_direct_60deg.xlsx
@@ -382,7 +382,7 @@
         <v>-0.4875</v>
       </c>
       <c r="B2">
-        <v>-501.8642238104799</v>
+        <v>-468.5457716930114</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -390,7 +390,7 @@
         <v>-0.4776515151515152</v>
       </c>
       <c r="B3">
-        <v>-499.5404033536049</v>
+        <v>-466.2219512361364</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -398,7 +398,7 @@
         <v>-0.4678030303030303</v>
       </c>
       <c r="B4">
-        <v>-497.21658289673</v>
+        <v>-463.8981307792615</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -406,7 +406,7 @@
         <v>-0.4579545454545455</v>
       </c>
       <c r="B5">
-        <v>-494.8927624398549</v>
+        <v>-461.5743103223865</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -414,7 +414,7 @@
         <v>-0.4481060606060606</v>
       </c>
       <c r="B6">
-        <v>-492.56894198298</v>
+        <v>-459.2504898655114</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -422,7 +422,7 @@
         <v>-0.4382575757575758</v>
       </c>
       <c r="B7">
-        <v>-490.245121526105</v>
+        <v>-456.9266694086365</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -430,7 +430,7 @@
         <v>-0.428409090909091</v>
       </c>
       <c r="B8">
-        <v>-487.92130106923</v>
+        <v>-454.6028489517615</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -438,7 +438,7 @@
         <v>-0.4185606060606061</v>
       </c>
       <c r="B9">
-        <v>-485.597480612355</v>
+        <v>-452.2790284948865</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -446,7 +446,7 @@
         <v>-0.4087121212121212</v>
       </c>
       <c r="B10">
-        <v>-483.27366015548</v>
+        <v>-449.9552080380116</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -454,7 +454,7 @@
         <v>-0.3988636363636364</v>
       </c>
       <c r="B11">
-        <v>-480.9498396986051</v>
+        <v>-447.6313875811366</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -462,7 +462,7 @@
         <v>-0.3890151515151515</v>
       </c>
       <c r="B12">
-        <v>-478.62601924173</v>
+        <v>-445.3075671242617</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -470,7 +470,7 @@
         <v>-0.3791666666666667</v>
       </c>
       <c r="B13">
-        <v>-476.3021987848551</v>
+        <v>-442.9837466673866</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -478,7 +478,7 @@
         <v>-0.3693181818181819</v>
       </c>
       <c r="B14">
-        <v>-473.9783783279803</v>
+        <v>-440.6599262105117</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -486,7 +486,7 @@
         <v>-0.359469696969697</v>
       </c>
       <c r="B15">
-        <v>-471.6545578711052</v>
+        <v>-438.3361057536366</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -494,7 +494,7 @@
         <v>-0.3496212121212122</v>
       </c>
       <c r="B16">
-        <v>-469.3307374142303</v>
+        <v>-436.0122852967617</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -502,7 +502,7 @@
         <v>-0.3397727272727273</v>
       </c>
       <c r="B17">
-        <v>-467.0069169573552</v>
+        <v>-433.6884648398867</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -510,7 +510,7 @@
         <v>-0.3299242424242425</v>
       </c>
       <c r="B18">
-        <v>-464.6830965004801</v>
+        <v>-431.3646443830116</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -518,7 +518,7 @@
         <v>-0.3200757575757576</v>
       </c>
       <c r="B19">
-        <v>-462.3592760436053</v>
+        <v>-429.0408239261367</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -526,7 +526,7 @@
         <v>-0.3102272727272727</v>
       </c>
       <c r="B20">
-        <v>-460.0354555867303</v>
+        <v>-426.7170034692617</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -534,7 +534,7 @@
         <v>-0.3003787878787879</v>
       </c>
       <c r="B21">
-        <v>-457.7116351298553</v>
+        <v>-424.3931830123868</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -542,7 +542,7 @@
         <v>-0.290530303030303</v>
       </c>
       <c r="B22">
-        <v>-455.3878146729803</v>
+        <v>-422.0693625555118</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -550,7 +550,7 @@
         <v>-0.2806818181818182</v>
       </c>
       <c r="B23">
-        <v>-453.0639942161054</v>
+        <v>-419.7455420986369</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -558,7 +558,7 @@
         <v>-0.2708333333333334</v>
       </c>
       <c r="B24">
-        <v>-450.7401737592303</v>
+        <v>-417.4217216417618</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -566,7 +566,7 @@
         <v>-0.2609848484848485</v>
       </c>
       <c r="B25">
-        <v>-448.4163533023553</v>
+        <v>-415.0979011848869</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -574,7 +574,7 @@
         <v>-0.2511363636363637</v>
       </c>
       <c r="B26">
-        <v>-446.0925328454804</v>
+        <v>-412.7740807280118</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -582,7 +582,7 @@
         <v>-0.2412878787878788</v>
       </c>
       <c r="B27">
-        <v>-443.7687123886055</v>
+        <v>-410.4502602711369</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -590,7 +590,7 @@
         <v>-0.2314393939393939</v>
       </c>
       <c r="B28">
-        <v>-441.4448919317304</v>
+        <v>-408.1264398142619</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -598,7 +598,7 @@
         <v>-0.2215909090909091</v>
       </c>
       <c r="B29">
-        <v>-439.1210714748555</v>
+        <v>-405.802619357387</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -606,7 +606,7 @@
         <v>-0.2117424242424243</v>
       </c>
       <c r="B30">
-        <v>-436.7972510179804</v>
+        <v>-403.4787989005119</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -614,7 +614,7 @@
         <v>-0.2018939393939394</v>
       </c>
       <c r="B31">
-        <v>-434.4734305611054</v>
+        <v>-401.154978443637</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -622,7 +622,7 @@
         <v>-0.1920454545454546</v>
       </c>
       <c r="B32">
-        <v>-432.1496101042305</v>
+        <v>-398.831157986762</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -630,7 +630,7 @@
         <v>-0.1821969696969697</v>
       </c>
       <c r="B33">
-        <v>-429.8257896473555</v>
+        <v>-396.507337529887</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -638,7 +638,7 @@
         <v>-0.1723484848484849</v>
       </c>
       <c r="B34">
-        <v>-427.5019691904805</v>
+        <v>-394.183517073012</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -646,7 +646,7 @@
         <v>-0.1625</v>
       </c>
       <c r="B35">
-        <v>-425.1781487336055</v>
+        <v>-391.8596966161369</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -654,7 +654,7 @@
         <v>-0.1526515151515151</v>
       </c>
       <c r="B36">
-        <v>-422.8543282767305</v>
+        <v>-389.535876159262</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -662,7 +662,7 @@
         <v>-0.1428030303030303</v>
       </c>
       <c r="B37">
-        <v>-420.5305078198554</v>
+        <v>-387.2120557023871</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -670,7 +670,7 @@
         <v>-0.1329545454545454</v>
       </c>
       <c r="B38">
-        <v>-418.2066873629806</v>
+        <v>-384.8882352455121</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -678,7 +678,7 @@
         <v>-0.1231060606060606</v>
       </c>
       <c r="B39">
-        <v>-415.8828669061056</v>
+        <v>-382.5644147886371</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -686,7 +686,7 @@
         <v>-0.1132575757575758</v>
       </c>
       <c r="B40">
-        <v>-413.5590464492307</v>
+        <v>-380.2405943317622</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -694,7 +694,7 @@
         <v>-0.1034090909090909</v>
       </c>
       <c r="B41">
-        <v>-411.2352259923557</v>
+        <v>-377.9167738748871</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -702,7 +702,7 @@
         <v>-0.09356060606060607</v>
       </c>
       <c r="B42">
-        <v>-408.9114055354806</v>
+        <v>-375.5929534180121</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -710,7 +710,7 @@
         <v>-0.08371212121212124</v>
       </c>
       <c r="B43">
-        <v>-406.5875850786057</v>
+        <v>-373.2691329611371</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -718,7 +718,7 @@
         <v>-0.07386363636363635</v>
       </c>
       <c r="B44">
-        <v>-404.2637646217307</v>
+        <v>-370.9453125042621</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -726,7 +726,7 @@
         <v>-0.06401515151515152</v>
       </c>
       <c r="B45">
-        <v>-401.9399441648557</v>
+        <v>-368.6214920473873</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -734,7 +734,7 @@
         <v>-0.0541666666666667</v>
       </c>
       <c r="B46">
-        <v>-399.6161237079808</v>
+        <v>-366.2976715905123</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -742,7 +742,7 @@
         <v>-0.04431818181818181</v>
       </c>
       <c r="B47">
-        <v>-397.2923032511057</v>
+        <v>-363.9738511336373</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -750,7 +750,7 @@
         <v>-0.03446969696969698</v>
       </c>
       <c r="B48">
-        <v>-394.9684827942308</v>
+        <v>-361.6500306767622</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -758,7 +758,7 @@
         <v>-0.0246212121212121</v>
       </c>
       <c r="B49">
-        <v>-392.6446623373558</v>
+        <v>-359.3262102198873</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -766,7 +766,7 @@
         <v>-0.01477272727272727</v>
       </c>
       <c r="B50">
-        <v>-390.3208418804809</v>
+        <v>-357.0023897630123</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -774,7 +774,7 @@
         <v>-0.004924242424242442</v>
       </c>
       <c r="B51">
-        <v>-387.9970214236058</v>
+        <v>-354.6785693061374</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -782,7 +782,7 @@
         <v>0.004924242424242442</v>
       </c>
       <c r="B52">
-        <v>-385.6732009667309</v>
+        <v>-352.3547488492624</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -790,7 +790,7 @@
         <v>0.01477272727272727</v>
       </c>
       <c r="B53">
-        <v>-383.3493805098558</v>
+        <v>-350.0309283923874</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -798,7 +798,7 @@
         <v>0.02462121212121215</v>
       </c>
       <c r="B54">
-        <v>-381.0255600529809</v>
+        <v>-347.7071079355125</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -806,7 +806,7 @@
         <v>0.03446969696969693</v>
       </c>
       <c r="B55">
-        <v>-378.701739596106</v>
+        <v>-345.3832874786375</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -814,7 +814,7 @@
         <v>0.04431818181818181</v>
       </c>
       <c r="B56">
-        <v>-376.3779191392309</v>
+        <v>-343.0594670217624</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -822,7 +822,7 @@
         <v>0.0541666666666667</v>
       </c>
       <c r="B57">
-        <v>-374.054098682356</v>
+        <v>-340.7356465648875</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -830,7 +830,7 @@
         <v>0.06401515151515147</v>
       </c>
       <c r="B58">
-        <v>-371.7302782254809</v>
+        <v>-338.4118261080124</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -838,7 +838,7 @@
         <v>0.07386363636363635</v>
       </c>
       <c r="B59">
-        <v>-369.4064577686059</v>
+        <v>-336.0880056511375</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -846,7 +846,7 @@
         <v>0.08371212121212124</v>
       </c>
       <c r="B60">
-        <v>-367.0826373117311</v>
+        <v>-333.7641851942625</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -854,7 +854,7 @@
         <v>0.09356060606060612</v>
       </c>
       <c r="B61">
-        <v>-364.758816854856</v>
+        <v>-331.4403647373874</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -862,7 +862,7 @@
         <v>0.1034090909090909</v>
       </c>
       <c r="B62">
-        <v>-362.4349963979811</v>
+        <v>-329.1165442805126</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -870,7 +870,7 @@
         <v>0.1132575757575758</v>
       </c>
       <c r="B63">
-        <v>-360.1111759411061</v>
+        <v>-326.7927238236376</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -878,7 +878,7 @@
         <v>0.1231060606060607</v>
       </c>
       <c r="B64">
-        <v>-357.7873554842312</v>
+        <v>-324.4689033667626</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -886,7 +886,7 @@
         <v>0.1329545454545454</v>
       </c>
       <c r="B65">
-        <v>-355.4635350273561</v>
+        <v>-322.1450829098876</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -894,7 +894,7 @@
         <v>0.1428030303030303</v>
       </c>
       <c r="B66">
-        <v>-353.1397145704811</v>
+        <v>-319.8212624530125</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -902,7 +902,7 @@
         <v>0.1526515151515152</v>
       </c>
       <c r="B67">
-        <v>-350.8158941136062</v>
+        <v>-317.4974419961376</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -910,7 +910,7 @@
         <v>0.1625</v>
       </c>
       <c r="B68">
-        <v>-348.4920736567311</v>
+        <v>-315.1736215392627</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -918,7 +918,7 @@
         <v>0.1723484848484849</v>
       </c>
       <c r="B69">
-        <v>-346.1682531998562</v>
+        <v>-312.8498010823877</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -926,7 +926,7 @@
         <v>0.1821969696969697</v>
       </c>
       <c r="B70">
-        <v>-343.8444327429811</v>
+        <v>-310.5259806255126</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -934,7 +934,7 @@
         <v>0.1920454545454545</v>
       </c>
       <c r="B71">
-        <v>-341.5206122861063</v>
+        <v>-308.2021601686377</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -942,7 +942,7 @@
         <v>0.2018939393939394</v>
       </c>
       <c r="B72">
-        <v>-339.1967918292312</v>
+        <v>-305.8783397117628</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -950,7 +950,7 @@
         <v>0.2117424242424243</v>
       </c>
       <c r="B73">
-        <v>-336.8729713723563</v>
+        <v>-303.5545192548877</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -958,7 +958,7 @@
         <v>0.2215909090909092</v>
       </c>
       <c r="B74">
-        <v>-334.5491509154813</v>
+        <v>-301.2306987980128</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -966,7 +966,7 @@
         <v>0.2314393939393939</v>
       </c>
       <c r="B75">
-        <v>-332.2253304586063</v>
+        <v>-298.9068783411378</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -974,7 +974,7 @@
         <v>0.2412878787878788</v>
       </c>
       <c r="B76">
-        <v>-329.9015100017313</v>
+        <v>-296.5830578842628</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -982,7 +982,7 @@
         <v>0.2511363636363637</v>
       </c>
       <c r="B77">
-        <v>-327.5776895448563</v>
+        <v>-294.2592374273879</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -990,7 +990,7 @@
         <v>0.2609848484848485</v>
       </c>
       <c r="B78">
-        <v>-325.2538690879814</v>
+        <v>-291.9354169705129</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -998,7 +998,7 @@
         <v>0.2708333333333334</v>
       </c>
       <c r="B79">
-        <v>-322.9300486311064</v>
+        <v>-289.6115965136378</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1006,7 +1006,7 @@
         <v>0.2806818181818183</v>
       </c>
       <c r="B80">
-        <v>-320.6062281742314</v>
+        <v>-287.2877760567629</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1014,7 +1014,7 @@
         <v>0.290530303030303</v>
       </c>
       <c r="B81">
-        <v>-318.2824077173563</v>
+        <v>-284.963955599888</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1022,7 +1022,7 @@
         <v>0.3003787878787879</v>
       </c>
       <c r="B82">
-        <v>-315.9585872604815</v>
+        <v>-282.6401351430129</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1030,7 +1030,7 @@
         <v>0.3102272727272728</v>
       </c>
       <c r="B83">
-        <v>-313.6347668036066</v>
+        <v>-280.316314686138</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1038,7 +1038,7 @@
         <v>0.3200757575757576</v>
       </c>
       <c r="B84">
-        <v>-311.3109463467315</v>
+        <v>-277.9924942292629</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1046,7 +1046,7 @@
         <v>0.3299242424242425</v>
       </c>
       <c r="B85">
-        <v>-308.9871258898565</v>
+        <v>-275.668673772388</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1054,7 +1054,7 @@
         <v>0.3397727272727273</v>
       </c>
       <c r="B86">
-        <v>-306.6633054329815</v>
+        <v>-273.344853315513</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1062,7 +1062,7 @@
         <v>0.3496212121212121</v>
       </c>
       <c r="B87">
-        <v>-304.3394849761066</v>
+        <v>-271.021032858638</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -1070,7 +1070,7 @@
         <v>0.359469696969697</v>
       </c>
       <c r="B88">
-        <v>-302.0156645192316</v>
+        <v>-268.6972124017631</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -1078,7 +1078,7 @@
         <v>0.3693181818181819</v>
       </c>
       <c r="B89">
-        <v>-299.6918440623565</v>
+        <v>-266.373391944888</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -1086,7 +1086,7 @@
         <v>0.3791666666666667</v>
       </c>
       <c r="B90">
-        <v>-297.3680236054817</v>
+        <v>-264.049571488013</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -1094,7 +1094,7 @@
         <v>0.3890151515151515</v>
       </c>
       <c r="B91">
-        <v>-295.0442031486066</v>
+        <v>-261.7257510311381</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -1102,7 +1102,7 @@
         <v>0.3988636363636364</v>
       </c>
       <c r="B92">
-        <v>-292.7203826917316</v>
+        <v>-259.401930574263</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -1110,7 +1110,7 @@
         <v>0.4087121212121213</v>
       </c>
       <c r="B93">
-        <v>-290.3965622348566</v>
+        <v>-257.0781101173881</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -1118,7 +1118,7 @@
         <v>0.4185606060606061</v>
       </c>
       <c r="B94">
-        <v>-288.0727417779816</v>
+        <v>-254.7542896605132</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -1126,7 +1126,7 @@
         <v>0.428409090909091</v>
       </c>
       <c r="B95">
-        <v>-285.7489213211067</v>
+        <v>-252.4304692036382</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -1134,7 +1134,7 @@
         <v>0.4382575757575758</v>
       </c>
       <c r="B96">
-        <v>-283.4251008642317</v>
+        <v>-250.1066487467632</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -1142,7 +1142,7 @@
         <v>0.4481060606060606</v>
       </c>
       <c r="B97">
-        <v>-281.1012804073567</v>
+        <v>-247.7828282898882</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -1150,7 +1150,7 @@
         <v>0.4579545454545455</v>
       </c>
       <c r="B98">
-        <v>-278.7774599504817</v>
+        <v>-245.4590078330131</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -1158,7 +1158,7 @@
         <v>0.4678030303030304</v>
       </c>
       <c r="B99">
-        <v>-276.4536394936067</v>
+        <v>-243.1351873761382</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -1166,7 +1166,7 @@
         <v>0.4776515151515152</v>
       </c>
       <c r="B100">
-        <v>-274.1298190367318</v>
+        <v>-240.8113669192632</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -1174,7 +1174,7 @@
         <v>0.4875</v>
       </c>
       <c r="B101">
-        <v>-271.8059985798568</v>
+        <v>-238.4875464623882</v>
       </c>
     </row>
   </sheetData>

</xml_diff>